<commit_message>
fix docs: erd menyesuaikan fitur
</commit_message>
<xml_diff>
--- a/docs/erd_loan_approval.xlsx
+++ b/docs/erd_loan_approval.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tubes\eval-efishery\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B52EE5FB-E2D2-4343-848C-86ED0ACD7C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD78B2F-A9DA-4019-B07D-75A5E1F6EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8D2C07D4-D00F-4380-8505-23CDCD7BB484}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{8D2C07D4-D00F-4380-8505-23CDCD7BB484}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Loan" sheetId="2" r:id="rId2"/>
     <sheet name="Document" sheetId="3" r:id="rId3"/>
     <sheet name="LoanApplication" sheetId="7" r:id="rId4"/>
+    <sheet name="Account" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>userID</t>
   </si>
@@ -132,6 +133,18 @@
   </si>
   <si>
     <t>User(userID)</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Account(username)</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -492,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FC9CD6-DB37-4ACD-89C1-4B71F9C08267}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +565,20 @@
       </c>
       <c r="B6" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545146E9-CEE4-49EE-977C-5A214024A105}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -749,4 +776,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342414E7-3395-4FFF-99DC-B22DB926AC75}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update readme and erd adjustment
</commit_message>
<xml_diff>
--- a/docs/erd_loan_approval.xlsx
+++ b/docs/erd_loan_approval.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tubes\eval-efishery\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD78B2F-A9DA-4019-B07D-75A5E1F6EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E790D-FECA-4C46-879C-EC18F39E8115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{8D2C07D4-D00F-4380-8505-23CDCD7BB484}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>userID</t>
   </si>
@@ -45,9 +45,6 @@
     <t>fullName</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>interest</t>
   </si>
   <si>
@@ -145,6 +139,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -505,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FC9CD6-DB37-4ACD-89C1-4B71F9C08267}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,13 +515,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,15 +529,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,29 +553,21 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -588,55 +577,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797A34C2-A838-4998-8336-79629CEB10FB}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -656,54 +653,54 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +713,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,51 +723,51 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -783,36 +780,36 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>